<commit_message>
Added knowledge base, improved prompts
</commit_message>
<xml_diff>
--- a/backend/data/portfolios.xlsx
+++ b/backend/data/portfolios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PortfollioAgent\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147E740D-CBF6-46C5-BE5C-8BC3401E2E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194F45C0-F98C-4E3C-8E13-71533C4CF9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{09DE11FB-184F-4121-AFE5-3D32D456FF9A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{09DE11FB-184F-4121-AFE5-3D32D456FF9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Potfolios" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
@@ -741,7 +741,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="165">
   <si>
     <t>client_id</t>
   </si>
@@ -1224,6 +1224,18 @@
   </si>
   <si>
     <t>Purchase Price</t>
+  </si>
+  <si>
+    <t>market_cap_bucket</t>
+  </si>
+  <si>
+    <t>Large Cap</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Mid Cap</t>
   </si>
 </sst>
 </file>
@@ -1231,12 +1243,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-14009]yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="[$-14009]yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1250,7 +1268,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1258,13 +1276,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1970,10 +2007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB5E37E-00E6-4924-94C5-EA4B575A533F}">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1988,7 +2025,7 @@
     <col min="8" max="8" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2013,8 +2050,11 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2039,8 +2079,11 @@
       <c r="H2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2065,8 +2108,11 @@
       <c r="H3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2091,8 +2137,11 @@
       <c r="H4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2117,8 +2166,11 @@
       <c r="H5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2143,8 +2195,11 @@
       <c r="H6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2169,8 +2224,11 @@
       <c r="H7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -2195,8 +2253,11 @@
       <c r="H8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -2221,8 +2282,11 @@
       <c r="H9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -2247,8 +2311,11 @@
       <c r="H10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -2273,8 +2340,11 @@
       <c r="H11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -2299,8 +2369,11 @@
       <c r="H12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2325,8 +2398,11 @@
       <c r="H13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2351,8 +2427,11 @@
       <c r="H14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -2377,8 +2456,11 @@
       <c r="H15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2403,8 +2485,11 @@
       <c r="H16" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -2429,8 +2514,11 @@
       <c r="H17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -2455,8 +2543,11 @@
       <c r="H18" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -2481,8 +2572,11 @@
       <c r="H19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -2507,8 +2601,11 @@
       <c r="H20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -2533,8 +2630,11 @@
       <c r="H21" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -2559,8 +2659,11 @@
       <c r="H22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -2585,8 +2688,11 @@
       <c r="H23" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -2611,8 +2717,11 @@
       <c r="H24" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -2637,8 +2746,11 @@
       <c r="H25" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -2663,8 +2775,11 @@
       <c r="H26" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -2689,8 +2804,11 @@
       <c r="H27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -2715,8 +2833,11 @@
       <c r="H28" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -2741,8 +2862,11 @@
       <c r="H29" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -2767,8 +2891,11 @@
       <c r="H30" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -2793,8 +2920,11 @@
       <c r="H31" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -2819,8 +2949,11 @@
       <c r="H32" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -2845,8 +2978,11 @@
       <c r="H33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -2871,8 +3007,11 @@
       <c r="H34" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -2897,8 +3036,11 @@
       <c r="H35" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>78</v>
       </c>
@@ -2923,8 +3065,11 @@
       <c r="H36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -2949,8 +3094,11 @@
       <c r="H37" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -2975,8 +3123,11 @@
       <c r="H38" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>97</v>
       </c>
@@ -3001,8 +3152,11 @@
       <c r="H39" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -3027,8 +3181,11 @@
       <c r="H40" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>97</v>
       </c>
@@ -3053,8 +3210,11 @@
       <c r="H41" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>97</v>
       </c>
@@ -3079,8 +3239,11 @@
       <c r="H42" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -3105,8 +3268,11 @@
       <c r="H43" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>97</v>
       </c>
@@ -3131,8 +3297,11 @@
       <c r="H44" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I44" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>97</v>
       </c>
@@ -3157,8 +3326,11 @@
       <c r="H45" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I45" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -3183,8 +3355,11 @@
       <c r="H46" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>117</v>
       </c>
@@ -3209,8 +3384,11 @@
       <c r="H47" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I47" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>117</v>
       </c>
@@ -3235,8 +3413,11 @@
       <c r="H48" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I48" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>117</v>
       </c>
@@ -3261,8 +3442,11 @@
       <c r="H49" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I49" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>117</v>
       </c>
@@ -3287,8 +3471,11 @@
       <c r="H50" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I50" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>117</v>
       </c>
@@ -3313,8 +3500,11 @@
       <c r="H51" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I51" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>117</v>
       </c>
@@ -3339,8 +3529,11 @@
       <c r="H52" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I52" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>117</v>
       </c>
@@ -3365,8 +3558,11 @@
       <c r="H53" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>117</v>
       </c>
@@ -3391,8 +3587,11 @@
       <c r="H54" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I54" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>117</v>
       </c>
@@ -3417,8 +3616,11 @@
       <c r="H55" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I55" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>117</v>
       </c>
@@ -3443,8 +3645,11 @@
       <c r="H56" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -3469,8 +3674,11 @@
       <c r="H57" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I57" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>136</v>
       </c>
@@ -3495,8 +3703,11 @@
       <c r="H58" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I58" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>136</v>
       </c>
@@ -3521,8 +3732,11 @@
       <c r="H59" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I59" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>136</v>
       </c>
@@ -3547,8 +3761,11 @@
       <c r="H60" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I60" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>136</v>
       </c>
@@ -3573,8 +3790,11 @@
       <c r="H61" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I61" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>136</v>
       </c>
@@ -3599,8 +3819,11 @@
       <c r="H62" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I62" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>136</v>
       </c>
@@ -3625,8 +3848,11 @@
       <c r="H63" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I63" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>136</v>
       </c>
@@ -3651,8 +3877,11 @@
       <c r="H64" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I64" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>136</v>
       </c>
@@ -3677,8 +3906,11 @@
       <c r="H65" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I65" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>136</v>
       </c>
@@ -3703,8 +3935,11 @@
       <c r="H66" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I66" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>136</v>
       </c>
@@ -3729,8 +3964,11 @@
       <c r="H67" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>136</v>
       </c>
@@ -3755,8 +3993,11 @@
       <c r="H68" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I68" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -3781,8 +4022,11 @@
       <c r="H69" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I69" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>136</v>
       </c>
@@ -3806,11 +4050,15 @@
       </c>
       <c r="H70" t="s">
         <v>31</v>
+      </c>
+      <c r="I70" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H70" xr:uid="{AAB5E37E-00E6-4924-94C5-EA4B575A533F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>